<commit_message>
nuts2 rest sector basically done
</commit_message>
<xml_diff>
--- a/input/general/Efficiency_Combustion.xlsx
+++ b/input/general/Efficiency_Combustion.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAC326DF-B53A-4B41-A167-8FCD27D33DEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D2ACA75-DA45-4785-97B4-EAB90DCCFE83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="1140" windowWidth="21600" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30510" yWindow="-10575" windowWidth="25185" windowHeight="16890" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="72">
   <si>
     <t>Efficiency</t>
   </si>
@@ -246,6 +246,9 @@
   </si>
   <si>
     <t>Same efficiency as for waste</t>
+  </si>
+  <si>
+    <t>Brennstoff allgemein</t>
   </si>
 </sst>
 </file>
@@ -615,20 +618,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.140625" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1796875" customWidth="1"/>
+    <col min="3" max="3" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>37</v>
       </c>
@@ -645,7 +648,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -663,7 +666,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -678,7 +681,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>68</v>
       </c>
@@ -695,7 +698,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -712,7 +715,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -729,7 +732,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -744,7 +747,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -758,7 +761,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -775,7 +778,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -792,7 +795,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
         <v>21</v>
@@ -808,37 +811,51 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12">
+        <v>0.9</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
       <c r="B23" s="3"/>
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
       <c r="D24" s="3"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="1"/>
     </row>
   </sheetData>
@@ -848,20 +865,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2C57BA3-29DC-44DD-BD94-7E5A2ED8761D}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>37</v>
       </c>
@@ -875,7 +892,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -889,7 +906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -901,7 +918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>68</v>
       </c>
@@ -913,7 +930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -927,7 +944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -941,7 +958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -953,7 +970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -964,7 +981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -978,7 +995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -992,7 +1009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
         <v>21</v>
@@ -1002,6 +1019,17 @@
         <v>1</v>
       </c>
       <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
         <v>0</v>
       </c>
     </row>
@@ -1018,15 +1046,15 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
-    <col min="3" max="3" width="64.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.81640625" customWidth="1"/>
+    <col min="3" max="3" width="64.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>41</v>
       </c>
@@ -1037,7 +1065,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B2" s="6" t="s">
         <v>44</v>
       </c>
@@ -1045,7 +1073,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -1053,7 +1081,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -1067,7 +1095,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>28</v>
       </c>
@@ -1081,7 +1109,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>31</v>
       </c>
@@ -1095,10 +1123,10 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -1110,7 +1138,7 @@
       </c>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>53</v>
       </c>
@@ -1119,7 +1147,7 @@
       </c>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>61</v>
       </c>
@@ -1128,7 +1156,7 @@
       </c>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>63</v>
       </c>
@@ -1137,13 +1165,13 @@
       </c>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="C14" s="3" t="s">
         <v>62</v>
       </c>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>69</v>
       </c>
@@ -1152,12 +1180,12 @@
       </c>
       <c r="F15" s="5"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C16" s="3"/>
       <c r="E16" s="1"/>
       <c r="F16" s="5"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>48</v>
       </c>
@@ -1171,11 +1199,11 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B18" s="4"/>
       <c r="C18" s="5"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>40</v>
       </c>
@@ -1189,7 +1217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C20" t="s">
         <v>32</v>
       </c>
@@ -1197,7 +1225,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C21" t="s">
         <v>33</v>
       </c>
@@ -1205,7 +1233,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C22" t="s">
         <v>25</v>
       </c>
@@ -1213,7 +1241,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C23" t="s">
         <v>23</v>
       </c>
@@ -1221,7 +1249,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C24" t="s">
         <v>26</v>
       </c>
@@ -1229,28 +1257,28 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
       <c r="B26" s="3"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="1"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="7"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="7"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="1"/>
       <c r="G30" s="1"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="G32" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
written groups in sheet and implemented fuel efficiency and substitution
</commit_message>
<xml_diff>
--- a/input/general/Efficiency_Combustion.xlsx
+++ b/input/general/Efficiency_Combustion.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D2ACA75-DA45-4785-97B4-EAB90DCCFE83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75846663-8EC9-4795-86D3-C5B194BA4591}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30510" yWindow="-10575" windowWidth="25185" windowHeight="16890" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="73">
   <si>
     <t>Efficiency</t>
   </si>
@@ -249,6 +249,9 @@
   </si>
   <si>
     <t>Brennstoff allgemein</t>
+  </si>
+  <si>
+    <t>0.9</t>
   </si>
 </sst>
 </file>
@@ -337,8 +340,8 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -622,7 +625,7 @@
       <selection activeCell="A12" sqref="A12:E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="21.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.1796875" customWidth="1"/>
@@ -868,10 +871,10 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="21.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.54296875" bestFit="1" customWidth="1"/>
@@ -1026,8 +1029,8 @@
       <c r="A12" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C12">
-        <v>1</v>
+      <c r="C12" t="s">
+        <v>72</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -1035,6 +1038,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1046,7 +1050,7 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="20.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.81640625" customWidth="1"/>

</xml_diff>